<commit_message>
Menambahkan materi Data Analyst, Data Scientist & Data Engineer.
</commit_message>
<xml_diff>
--- a/1-microsoft-excel/5-papan-tulis/papan-tulis.xlsx
+++ b/1-microsoft-excel/5-papan-tulis/papan-tulis.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\road-to-programmer\data-analyst-data-scientist-data-engineer\1-microsoft-excel\5-papan-tulis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C22FD84-59D3-46F0-AE97-AEE8720B7758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C433EB-00EC-4232-89FD-BFD3F702A974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="STD &amp; QUARTILE" sheetId="1" r:id="rId1"/>
+    <sheet name="CORREL &amp; VAR" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Tahun</t>
   </si>
@@ -59,13 +60,91 @@
   </si>
   <si>
     <t>STDEV.S</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Menghitung Nilai Kuartil</t>
+  </si>
+  <si>
+    <t>Nilai Minimum</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Nilai Maksimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korelasi Biaya Iklan dengan  Jumlah Penjualan </t>
+  </si>
+  <si>
+    <t>Bulan</t>
+  </si>
+  <si>
+    <t>Biaya Iklan</t>
+  </si>
+  <si>
+    <t>Jumlah Penjualan (unit)</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,8 +181,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +215,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -158,11 +265,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -180,12 +288,45 @@
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -461,177 +602,600 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F21"/>
+  <dimension ref="B3:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+    </row>
+    <row r="4" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>2002</v>
       </c>
       <c r="C4" s="1">
         <v>8.3900000000000002E-2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="6">
-        <f>STDEV(C4:C17)</f>
-        <v>0.35634313596511236</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+        <f>STDEV(C4:C23)</f>
+        <v>0.31131011886102122</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="6">
+        <f>STDEVA(C4:C27)</f>
+        <v>0.3063461102833106</v>
+      </c>
+      <c r="K4">
+        <v>50</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="7">
+        <f>_xlfn.QUARTILE.INC(K4:K28,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>2003</v>
       </c>
       <c r="C5" s="1">
         <v>0.62819999999999998</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F5" s="6">
+        <f>STDEVP(C4:C23)</f>
+        <v>0.30342757059964082</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <v>50</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="7">
+        <f>_xlfn.QUARTILE.INC(K4:K28,1)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>2004</v>
       </c>
       <c r="C6" s="1">
         <v>0.4456</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F6" s="6">
+        <f>STDEVA(C4:C23)</f>
+        <v>0.31131011886102122</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="6">
+        <f>STDEVA(C4:C27)</f>
+        <v>0.3063461102833106</v>
+      </c>
+      <c r="K6">
+        <v>28</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="7">
+        <f>_xlfn.QUARTILE.INC(K4:K28,2)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>2005</v>
       </c>
       <c r="C7" s="1">
         <v>0.16239999999999999</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F7" s="6">
+        <f>STDEVPA(C4:C23)</f>
+        <v>0.30342757059964082</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>31</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="7">
+        <f>_xlfn.QUARTILE.INC(K4:K28,3)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>2006</v>
       </c>
       <c r="C8" s="1">
         <v>0.55300000000000005</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F8" s="6">
+        <f>_xlfn.STDEV.P(C4:C23)</f>
+        <v>0.30342757059964082</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8">
+        <v>46</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="7">
+        <f>_xlfn.QUARTILE.INC(K4:K28,4)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>2007</v>
       </c>
       <c r="C9" s="1">
         <v>0.52080000000000004</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F9" s="6">
+        <f>_xlfn.STDEV.S(C4:C23)</f>
+        <v>0.31131011886102122</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="6">
+        <f>_xlfn.STDEV.S(C4:C27)</f>
+        <v>0.3063461102833106</v>
+      </c>
+      <c r="K9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>2008</v>
       </c>
       <c r="C10" s="2">
         <v>-0.50639999999999996</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>2009</v>
       </c>
       <c r="C11" s="1">
         <v>0.86980000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>2010</v>
       </c>
       <c r="C12" s="1">
         <v>0.46129999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>2011</v>
       </c>
       <c r="C13" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>2012</v>
       </c>
       <c r="C14" s="1">
         <v>0.12939999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>2013</v>
       </c>
       <c r="C15" s="2">
         <v>-9.7999999999999997E-3</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>26</v>
+      </c>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+    </row>
+    <row r="16" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>2014</v>
       </c>
       <c r="C16" s="1">
         <v>0.22289999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>2015</v>
       </c>
       <c r="C17" s="2">
         <v>-0.12130000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="5">
+      <c r="K17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>2016</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.1532</v>
+      </c>
+      <c r="K18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>2017</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.19989999999999999</v>
+      </c>
+      <c r="K19">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>2018</v>
+      </c>
+      <c r="C20" s="1">
+        <v>-2.5399999999999999E-2</v>
+      </c>
+      <c r="K20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>2019</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>2020</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-5.0900000000000001E-2</v>
+      </c>
+      <c r="K22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="8">
+        <v>2021</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.1008</v>
+      </c>
+      <c r="K23">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="5">
+      <c r="C24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="5">
+      <c r="K25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="5">
+      <c r="K26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
         <v>2025</v>
       </c>
+      <c r="K27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M3:O3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C4:C24">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D72A709-EC0A-4CE7-9E5A-5299981813F7}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="16">
+        <v>500000</v>
+      </c>
+      <c r="C3" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="16">
+        <v>600000</v>
+      </c>
+      <c r="C4" s="7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="16">
+        <v>400000</v>
+      </c>
+      <c r="C5" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="16">
+        <v>800000</v>
+      </c>
+      <c r="C6" s="7">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="16">
+        <v>900000</v>
+      </c>
+      <c r="C7" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="16">
+        <v>1000000</v>
+      </c>
+      <c r="C8" s="7">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="16">
+        <v>550000</v>
+      </c>
+      <c r="C9" s="7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="16">
+        <v>700000</v>
+      </c>
+      <c r="C10" s="7">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="16">
+        <v>800000</v>
+      </c>
+      <c r="C11" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="16">
+        <v>500000</v>
+      </c>
+      <c r="C12" s="7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="16">
+        <v>1000000</v>
+      </c>
+      <c r="C13" s="7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="16">
+        <v>900000</v>
+      </c>
+      <c r="C14" s="7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="16">
+        <v>800000</v>
+      </c>
+      <c r="C15" s="7">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>